<commit_message>
Train val curve plots
</commit_message>
<xml_diff>
--- a/results/Effisegnet results.xlsx
+++ b/results/Effisegnet results.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor\Documents\GitHub\tcc-effisegnet\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A78C965-E657-4C16-8895-82DC83E955B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901B556B-9BAF-4F12-B649-460D9B315444}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7830" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>N fold</t>
   </si>
@@ -76,7 +77,7 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>Digerença</t>
+    <t>Diferença</t>
   </si>
 </sst>
 </file>
@@ -86,9 +87,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="175" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -136,6 +137,27 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -147,6 +169,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -354,11 +377,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -394,45 +416,83 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="175" fontId="5" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Saída" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <numFmt numFmtId="175" formatCode="0.000"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF3F3F3F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF3F3F3F"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF3F3F3F"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF3F3F3F"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -468,6 +528,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="0.00000"/>
@@ -487,6 +548,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -553,9 +615,8 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color theme="1" tint="0.499984740745262"/>
+        <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -632,8 +693,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3472E310-2CD8-4621-B643-527E84A4EF56}" name="Tabela2" displayName="Tabela2" ref="J2:N8" totalsRowCount="1" headerRowDxfId="7">
-  <autoFilter ref="J2:N7" xr:uid="{89BF2B04-8149-4E74-BC3E-413EDC1AE37E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3472E310-2CD8-4621-B643-527E84A4EF56}" name="Tabela2" displayName="Tabela2" ref="A1:E7" totalsRowCount="1" headerRowDxfId="7">
+  <autoFilter ref="A1:E6" xr:uid="{89BF2B04-8149-4E74-BC3E-413EDC1AE37E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A377B230-823F-417F-ABEE-FCF56F18AE4D}" name="Métricas"/>
     <tableColumn id="2" xr3:uid="{F7FE22A2-D745-499B-A75B-DFD6D852C194}" name="Média" dataDxfId="6" totalsRowDxfId="3"/>
@@ -641,8 +702,8 @@
       <calculatedColumnFormula>STDEV(Table1[test_accuracy])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{3D5510CD-1136-4048-AFFC-C35C8829730D}" name="Kvasir-SEG" dataDxfId="4" totalsRowDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{56A3B460-BF91-4833-A959-827DCA06A57F}" name="Digerença" totalsRowFunction="custom" totalsRowDxfId="0" totalsRowCellStyle="Saída">
-      <totalsRowFormula>MEDIAN(N4:N7)</totalsRowFormula>
+    <tableColumn id="5" xr3:uid="{56A3B460-BF91-4833-A959-827DCA06A57F}" name="Diferença" totalsRowFunction="custom" totalsRowDxfId="0">
+      <totalsRowFormula>MEDIAN(E3:E6)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -850,11 +911,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -865,12 +926,12 @@
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="25" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
     <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -886,17 +947,17 @@
       <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -915,29 +976,14 @@
       <c r="F2" s="2">
         <v>0.83632951974868697</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="22">
         <v>0.86941820383071899</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="15">
         <v>0.45632398128509499</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -956,28 +1002,14 @@
       <c r="F3" s="4">
         <v>0.886846423149108</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="23">
         <v>0.89474707841873102</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="16">
         <v>0.37093949317932101</v>
       </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="13">
-        <f>AVERAGE(Table1[test_accuracy])</f>
-        <v>0.95838806629180873</v>
-      </c>
-      <c r="L3" s="14">
-        <f>STDEV(Table1[test_accuracy])</f>
-        <v>4.7226902804401935E-3</v>
-      </c>
-      <c r="M3" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -996,32 +1028,14 @@
       <c r="F4" s="6">
         <v>0.89069527387618996</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="22">
         <v>0.89822375774383501</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="15">
         <v>0.39095532894134499</v>
       </c>
-      <c r="J4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="13">
-        <f>AVERAGE(Table1[test_recall])</f>
-        <v>0.87931089997291534</v>
-      </c>
-      <c r="L4" s="14">
-        <f>STDEV(Table1[test_recall])</f>
-        <v>1.7179659375133185E-2</v>
-      </c>
-      <c r="M4" s="13">
-        <v>0.93679999999999997</v>
-      </c>
-      <c r="N4" s="26">
-        <f>(Tabela2[[#This Row],[Kvasir-SEG]]-Tabela2[[#This Row],[Média]])/Tabela2[[#This Row],[Kvasir-SEG]]</f>
-        <v>6.1367527782968223E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1040,32 +1054,14 @@
       <c r="F5" s="4">
         <v>0.85141932964324896</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="23">
         <v>0.88918739557266202</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="16">
         <v>0.42023080587387002</v>
       </c>
-      <c r="J5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="13">
-        <f>AVERAGE(Table1[test_precision])</f>
-        <v>0.90939586162567099</v>
-      </c>
-      <c r="L5" s="14">
-        <f>STDEV(Table1[test_precision])</f>
-        <v>3.0538533587015786E-2</v>
-      </c>
-      <c r="M5" s="13">
-        <v>0.94750000000000001</v>
-      </c>
-      <c r="N5" s="26">
-        <f>Tabela2[[#This Row],[Kvasir-SEG]]-Tabela2[[#This Row],[Média]]</f>
-        <v>3.8104138374329022E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1084,32 +1080,14 @@
       <c r="F6" s="6">
         <v>0.91606765985488803</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="22">
         <v>0.91964197158813399</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="15">
         <v>0.295303434133529</v>
       </c>
-      <c r="J6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="13">
-        <f>AVERAGE(Table1[test_iou])</f>
-        <v>0.7959846198558802</v>
-      </c>
-      <c r="L6" s="14">
-        <f>STDEV(Table1[test_iou])</f>
-        <v>4.2721180982942766E-2</v>
-      </c>
-      <c r="M6" s="13">
-        <v>0.87939999999999996</v>
-      </c>
-      <c r="N6" s="26">
-        <f>Tabela2[[#This Row],[Kvasir-SEG]]-Tabela2[[#This Row],[Média]]</f>
-        <v>8.3415380144119755E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1128,32 +1106,14 @@
       <c r="F7" s="4">
         <v>0.82969075441360396</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="23">
         <v>0.86972773075103704</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="16">
         <v>0.48123794794082603</v>
       </c>
-      <c r="J7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="13">
-        <f>AVERAGE(Table1[test_dice])</f>
-        <v>0.87875357866287163</v>
-      </c>
-      <c r="L7" s="14">
-        <f>STDEV(Table1[test_dice])</f>
-        <v>3.2630621403203809E-2</v>
-      </c>
-      <c r="M7" s="13">
-        <v>0.9304</v>
-      </c>
-      <c r="N7" s="26">
-        <f>Tabela2[[#This Row],[Kvasir-SEG]]-Tabela2[[#This Row],[Média]]</f>
-        <v>5.1646421337128379E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1172,21 +1132,14 @@
       <c r="F8" s="6">
         <v>0.91456949710845903</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="22">
         <v>0.91931194067001298</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="15">
         <v>0.32481867074966397</v>
       </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="27">
-        <f>MEDIAN(N4:N7)</f>
-        <v>5.6506974560048301E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1205,15 +1158,15 @@
       <c r="F9" s="4">
         <v>0.85750740766525202</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="23">
         <v>0.86778450012206998</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="16">
         <v>0.45104590058326699</v>
       </c>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1232,14 +1185,14 @@
       <c r="F10" s="6">
         <v>0.89235252141952504</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="22">
         <v>0.89455246925354004</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="15">
         <v>0.37025827169418302</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1258,12 +1211,15 @@
       <c r="F11" s="8">
         <v>0.91205739974975497</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="24">
         <v>0.91647171974182096</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="17">
         <v>0.29286625981330799</v>
       </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F15" s="27"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1273,9 +1229,165 @@
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4505BDCA-1059-4E91-B7A9-F3B479D9C170}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="13">
+        <f>AVERAGE(Table1[test_accuracy])</f>
+        <v>0.95838806629180873</v>
+      </c>
+      <c r="C2" s="14">
+        <f>STDEV(Table1[test_accuracy])</f>
+        <v>4.7226902804401935E-3</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="13">
+        <f>AVERAGE(Table1[test_recall])</f>
+        <v>0.87931089997291534</v>
+      </c>
+      <c r="C3" s="14">
+        <f>STDEV(Table1[test_recall])</f>
+        <v>1.7179659375133185E-2</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0.93679999999999997</v>
+      </c>
+      <c r="E3" s="21">
+        <f>(Tabela2[[#This Row],[Kvasir-SEG]]-Tabela2[[#This Row],[Média]])/Tabela2[[#This Row],[Kvasir-SEG]]</f>
+        <v>6.1367527782968223E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="13">
+        <f>AVERAGE(Table1[test_precision])</f>
+        <v>0.90939586162567099</v>
+      </c>
+      <c r="C4" s="14">
+        <f>STDEV(Table1[test_precision])</f>
+        <v>3.0538533587015786E-2</v>
+      </c>
+      <c r="D4" s="13">
+        <v>0.94750000000000001</v>
+      </c>
+      <c r="E4" s="21">
+        <f>Tabela2[[#This Row],[Kvasir-SEG]]-Tabela2[[#This Row],[Média]]</f>
+        <v>3.8104138374329022E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="13">
+        <f>AVERAGE(Table1[test_iou])</f>
+        <v>0.7959846198558802</v>
+      </c>
+      <c r="C5" s="14">
+        <f>STDEV(Table1[test_iou])</f>
+        <v>4.2721180982942766E-2</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.87939999999999996</v>
+      </c>
+      <c r="E5" s="21">
+        <f>Tabela2[[#This Row],[Kvasir-SEG]]-Tabela2[[#This Row],[Média]]</f>
+        <v>8.3415380144119755E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="13">
+        <f>AVERAGE(Table1[test_f1])</f>
+        <v>0.89390667676925628</v>
+      </c>
+      <c r="C6" s="14">
+        <f>STDEV(Table1[test_f1])</f>
+        <v>2.0345955027567982E-2</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0.9304</v>
+      </c>
+      <c r="E6" s="21">
+        <f>Tabela2[[#This Row],[Kvasir-SEG]]-Tabela2[[#This Row],[Média]]</f>
+        <v>3.6493323230743724E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="28"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="29">
+        <f>MEDIAN(E3:E6)</f>
+        <v>4.9735833078648622E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" s="12"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>